<commit_message>
lab4 + new бжд
</commit_message>
<xml_diff>
--- a/ОПД/4/трассировка.xlsx
+++ b/ОПД/4/трассировка.xlsx
@@ -5,15 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\docs_for_labs\ОПД\4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs_for_labs\docs_for_labs\ОПД\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="lab4_1" localSheetId="1">Лист2!$A$1:$L$47</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,8 +27,32 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="lab4" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="1251" sourceFile="D:\docs_for_labs\docs_for_labs\ОПД\4\lab4.csv" decimal="," thousands=" " comma="1">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="183">
   <si>
     <t>адр</t>
   </si>
@@ -318,6 +346,261 @@
   </si>
   <si>
     <t>JUMP P</t>
+  </si>
+  <si>
+    <t>комментарий</t>
+  </si>
+  <si>
+    <t>0-&gt;AC</t>
+  </si>
+  <si>
+    <t>AC-&gt;R</t>
+  </si>
+  <si>
+    <t>Y-&gt;AC</t>
+  </si>
+  <si>
+    <t>Z-&gt;AC</t>
+  </si>
+  <si>
+    <t>X-&gt;AC</t>
+  </si>
+  <si>
+    <t>AC+1-&gt;AC</t>
+  </si>
+  <si>
+    <t>AC-&gt;-(SP)</t>
+  </si>
+  <si>
+    <t>(SP)+ -&gt; AC</t>
+  </si>
+  <si>
+    <t>AC+R-&gt;AC</t>
+  </si>
+  <si>
+    <t>AC-R-&gt;AC</t>
+  </si>
+  <si>
+    <t>AC-1-&gt;AC</t>
+  </si>
+  <si>
+    <t>отключение тг</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Вызов п/п</t>
+  </si>
+  <si>
+    <t>Установить флаги по AC-A</t>
+  </si>
+  <si>
+    <t>Переход если &gt;= (знаковый)</t>
+  </si>
+  <si>
+    <t>AC+B-&gt;AC</t>
+  </si>
+  <si>
+    <t>GO TO P</t>
+  </si>
+  <si>
+    <t>Переход в J если N==1</t>
+  </si>
+  <si>
+    <t>A-&gt;AC</t>
+  </si>
+  <si>
+    <t>AC-ARG</t>
+  </si>
+  <si>
+    <t>ARG -&gt; AC</t>
+  </si>
+  <si>
+    <t>ARG + AC -&gt; AC</t>
+  </si>
+  <si>
+    <t>(SP)+-&gt;IP</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Знчн</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>NZVC</t>
+  </si>
+  <si>
+    <t>Адр</t>
+  </si>
+  <si>
+    <t>001A</t>
+  </si>
+  <si>
+    <t>FEA6</t>
+  </si>
+  <si>
+    <t>008B</t>
+  </si>
+  <si>
+    <t>FEA7</t>
+  </si>
+  <si>
+    <t>7FF</t>
+  </si>
+  <si>
+    <t>008C</t>
+  </si>
+  <si>
+    <t>7FE</t>
+  </si>
+  <si>
+    <t>008E</t>
+  </si>
+  <si>
+    <t>008F</t>
+  </si>
+  <si>
+    <t>01D6</t>
+  </si>
+  <si>
+    <t>000E</t>
+  </si>
+  <si>
+    <t>06FC</t>
+  </si>
+  <si>
+    <t>06FE</t>
+  </si>
+  <si>
+    <t>022C</t>
+  </si>
+  <si>
+    <t>000D</t>
+  </si>
+  <si>
+    <t>000C</t>
+  </si>
+  <si>
+    <t>5BB3</t>
+  </si>
+  <si>
+    <t>000A</t>
+  </si>
+  <si>
+    <t>5BB4</t>
+  </si>
+  <si>
+    <t>009A</t>
+  </si>
+  <si>
+    <t>009C</t>
+  </si>
+  <si>
+    <t>009D</t>
+  </si>
+  <si>
+    <t>01D4</t>
+  </si>
+  <si>
+    <t>00A0</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0116</t>
+  </si>
+  <si>
+    <t>0095</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>0305</t>
+  </si>
+  <si>
+    <t>0131</t>
+  </si>
+  <si>
+    <t>0307</t>
+  </si>
+  <si>
+    <t>0703</t>
+  </si>
+  <si>
+    <t>0088</t>
+  </si>
+  <si>
+    <t>0017</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>0704</t>
+  </si>
+  <si>
+    <t>0013</t>
+  </si>
+  <si>
+    <t>0012</t>
+  </si>
+  <si>
+    <t>0093</t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>0099</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>0004</t>
   </si>
 </sst>
 </file>
@@ -354,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,6 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -383,16 +667,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>473075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>73953</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>18198</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>156503</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>145198</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -409,8 +693,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8058150" y="57150"/>
-          <a:ext cx="17971428" cy="6819048"/>
+          <a:off x="12239625" y="0"/>
+          <a:ext cx="17971428" cy="6590448"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -420,6 +704,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lab4_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,23 +973,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.26953125" customWidth="1"/>
+    <col min="8" max="8" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,6 +1001,9 @@
       <c r="C1" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,8 +1013,11 @@
       <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -731,6 +1027,9 @@
       <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
@@ -740,8 +1039,11 @@
       <c r="G2" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -751,6 +1053,9 @@
       <c r="C3" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
@@ -760,8 +1065,11 @@
       <c r="G3" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -771,6 +1079,9 @@
       <c r="C4" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>33</v>
       </c>
@@ -780,8 +1091,11 @@
       <c r="G4" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -791,6 +1105,9 @@
       <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
@@ -800,8 +1117,11 @@
       <c r="G5" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -811,6 +1131,9 @@
       <c r="C6" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
@@ -820,8 +1143,11 @@
       <c r="G6" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -831,6 +1157,9 @@
       <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="E7" s="1">
         <v>700</v>
       </c>
@@ -840,8 +1169,11 @@
       <c r="G7" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -851,6 +1183,9 @@
       <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="E8" s="1">
         <v>701</v>
       </c>
@@ -860,8 +1195,11 @@
       <c r="G8" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -871,6 +1209,9 @@
       <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="E9" s="1">
         <v>702</v>
       </c>
@@ -880,8 +1221,11 @@
       <c r="G9" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -891,6 +1235,9 @@
       <c r="C10" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="E10" s="1">
         <v>703</v>
       </c>
@@ -900,8 +1247,11 @@
       <c r="G10" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -911,6 +1261,9 @@
       <c r="C11" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E11" s="1">
         <v>704</v>
       </c>
@@ -920,8 +1273,11 @@
       <c r="G11" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -931,6 +1287,9 @@
       <c r="C12" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E12" s="1">
         <v>705</v>
       </c>
@@ -940,8 +1299,11 @@
       <c r="G12" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -951,6 +1313,9 @@
       <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E13" s="1">
         <v>706</v>
       </c>
@@ -960,8 +1325,11 @@
       <c r="G13" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -971,8 +1339,11 @@
       <c r="C14" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -982,8 +1353,11 @@
       <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -993,8 +1367,11 @@
       <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1004,8 +1381,11 @@
       <c r="C17" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1015,8 +1395,11 @@
       <c r="C18" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1026,8 +1409,11 @@
       <c r="C19" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1037,8 +1423,11 @@
       <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1048,8 +1437,11 @@
       <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1059,8 +1451,11 @@
       <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1070,8 +1465,11 @@
       <c r="C23" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1081,8 +1479,11 @@
       <c r="C24" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1092,8 +1493,11 @@
       <c r="C25" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1103,8 +1507,11 @@
       <c r="C26" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1114,8 +1521,11 @@
       <c r="C27" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1125,8 +1535,11 @@
       <c r="C28" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1136,8 +1549,11 @@
       <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1146,6 +1562,9 @@
       </c>
       <c r="C30" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1153,4 +1572,1622 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection sqref="A1:L47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1796875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="5.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>702</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>702</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1">
+        <v>703</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1">
+        <v>705</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>703</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1">
+        <v>704</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>704</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="1">
+        <v>705</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1">
+        <v>700</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>700</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1">
+        <v>701</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="1">
+        <v>706</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>701</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1">
+        <v>703</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="1">
+        <v>701</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>703</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="1">
+        <v>704</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>704</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="1">
+        <v>705</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="1">
+        <v>702</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>702</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1">
+        <v>703</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="1">
+        <v>705</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>703</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="1">
+        <v>704</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>704</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>